<commit_message>
Pull together administrative shell documents
</commit_message>
<xml_diff>
--- a/admin_shell/budget_worksheet.xlsx
+++ b/admin_shell/budget_worksheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pschloss/Documents/Proposals/2020_RR_R25/admin_shell/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16AE2124-8FB3-564E-BA1D-40439E6FF5AB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDF2082E-4F2D-C049-BBAC-CDE11F25B33B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6520" yWindow="1820" windowWidth="25600" windowHeight="16060" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -80,7 +80,7 @@
     <t>Year 3</t>
   </si>
   <si>
-    <t>Assessment</t>
+    <t>Program evaluation</t>
   </si>
 </sst>
 </file>
@@ -646,7 +646,7 @@
   <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -814,13 +814,13 @@
         <v>15</v>
       </c>
       <c r="C12" s="1">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="D12" s="1">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="E12" s="1">
-        <v>1000</v>
+        <v>2000</v>
       </c>
       <c r="F12" s="1">
         <f>SUM(C12:E12)</f>
@@ -833,15 +833,15 @@
       </c>
       <c r="C14" s="1">
         <f>SUM(C7:C12)</f>
-        <v>74673</v>
+        <v>74173</v>
       </c>
       <c r="D14" s="1">
         <f>SUM(D7:D12)</f>
-        <v>76748.19</v>
+        <v>76248.19</v>
       </c>
       <c r="E14" s="1">
         <f>SUM(E7:E12)</f>
-        <v>78885.635699999999</v>
+        <v>79885.635699999999</v>
       </c>
       <c r="F14" s="1">
         <f>SUM(F7:F12)</f>
@@ -854,15 +854,15 @@
       </c>
       <c r="C15" s="1">
         <f>C14*0.08</f>
-        <v>5973.84</v>
+        <v>5933.84</v>
       </c>
       <c r="D15" s="1">
         <f>D14*0.08</f>
-        <v>6139.8552</v>
+        <v>6099.8552</v>
       </c>
       <c r="E15" s="1">
         <f>E14*0.08</f>
-        <v>6310.850856</v>
+        <v>6390.850856</v>
       </c>
       <c r="F15" s="1">
         <f>F14*0.08</f>
@@ -875,15 +875,15 @@
       </c>
       <c r="C16" s="1">
         <f>C15+C14</f>
-        <v>80646.84</v>
+        <v>80106.84</v>
       </c>
       <c r="D16" s="1">
         <f>D15+D14</f>
-        <v>82888.045200000008</v>
+        <v>82348.045200000008</v>
       </c>
       <c r="E16" s="1">
         <f>E15+E14</f>
-        <v>85196.486556000003</v>
+        <v>86276.486556000003</v>
       </c>
       <c r="F16" s="1">
         <f>F15+F14</f>

</xml_diff>